<commit_message>
(#128) Swissmedic import. Fix test
</commit_message>
<xml_diff>
--- a/test/data/xlsx/Packungen-2015.07.02.xlsx
+++ b/test/data/xlsx/Packungen-2015.07.02.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">{#name?}</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">{#name?}</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">{#NAME?}</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">{#NAME?}</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_1" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">sheet1!#ref!</definedName>
@@ -21,20 +21,31 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_1" vbProcedure="false">sheet1!#ref!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="104">
   <si>
-    <t>Zugelassene Packungen / Conditionnements autorisés</t>
+    <t xml:space="preserve">Zugelassene Packungen / Conditionnements autorisés</t>
   </si>
   <si>
-    <t>Stand / Etat au: 30.06.2015</t>
+    <t xml:space="preserve">Stand / Etat au: 30.06.2015</t>
   </si>
   <si>
     <r>
-      <t>* Die Gültigkeitsdauer entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten. Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen / 
+      <rPr>
+        <sz val="8.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">* Die Gültigkeitsdauer entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten. Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen / 
   La durée de validité correspond aux données figurant sur le certificat d'autorisation. Les autorisations provisoires, sans report de la date d'expiration, restent réservées. Tous les médicaments énumérés dans la liste sont autorisés au moment de la mise à jour de la liste. 
 **</t>
     </r>
@@ -46,7 +57,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Verzeichnisse</t>
+      <t xml:space="preserve">Verzeichnisse</t>
     </r>
     <r>
       <rPr>
@@ -55,7 +66,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(Kategorien der Kontrollmassnahmen, denen die Betäubungsmittel unterstellt sind) / Tableaux (catégories de mesures de contrôle auxquelles sont soumis les stupéfiants)
+      <t xml:space="preserve">(Kategorien der Kontrollmassnahmen, denen die Betäubungsmittel unterstellt sind) / Tableaux (catégories de mesures de contrôle auxquelles sont soumis les stupéfiants)
 a: Unterstehen allen Kontrollmassnahmen (s. auch Anhang a der BetmVV-EDI) / Soumis à toutes les mesures de contrôle (voir aussi le tableau a de l'OTStup-DFI)
 b: Unterstehen nicht allen Kontrollmassnahmen (s. auch Anhang b der BetmVV-EDI) / Soustraits partiellement au contrôle (voir aussi le tableau b de l'OTStup-DFI)
 c: Unterstehen nicht allen Kontrollmassnahmen; in kleinen Mengen ohne Verschreibung erhältlich (s. auch Verzeichnis c der BetmVV-EDI) / Soustraits partiellement au contrôle; pouvant être obtenus en petites quantités sans ordonnance (voir aussi le tableau c de l'OTStup-DFI)
@@ -63,329 +74,332 @@
     </r>
   </si>
   <si>
-    <t>Zulassungs-nummer
+    <t xml:space="preserve">Zulassungs-nummer
 Numéro d'autorisation</t>
   </si>
   <si>
-    <t>Dosisstärke-nummer
+    <t xml:space="preserve">Dosisstärke-nummer
 Numéro de dosage</t>
   </si>
   <si>
-    <t>Präparatebezeichnung  
+    <t xml:space="preserve">Präparatebezeichnung  
 Dénomination de la préparation</t>
   </si>
   <si>
-    <t>Zulassungsinhaberin
+    <t xml:space="preserve">Zulassungsinhaberin
 Titulaire de l'autorisation</t>
   </si>
   <si>
-    <t>Heilmittelcode
+    <t xml:space="preserve">Heilmittelcode
 Catégorie de la préparation</t>
   </si>
   <si>
-    <t>IT-Nummer
+    <t xml:space="preserve">IT-Nummer
 N° IT</t>
   </si>
   <si>
-    <t>ATC-Code
+    <t xml:space="preserve">ATC-Code
 Code ATC</t>
   </si>
   <si>
-    <t>Erstzulassungs-datum Präparat
+    <t xml:space="preserve">Erstzulassungs-datum Präparat
 Date de première autorisation de la préparation</t>
   </si>
   <si>
-    <t>Zul.datum Dosisstärke 
+    <t xml:space="preserve">Zul.datum Dosisstärke 
 Date d'autorisation du dosage</t>
   </si>
   <si>
-    <t>Gültigkeitsdauer der Zulassung * 
+    <t xml:space="preserve">Gültigkeitsdauer der Zulassung * 
 Durée de validité de l'AMM  *</t>
   </si>
   <si>
-    <t>Packungscode
+    <t xml:space="preserve">Packungscode
 Code d'emballage</t>
   </si>
   <si>
-    <t>Packungsgrösse
+    <t xml:space="preserve">Packungsgrösse
 Conditionnement</t>
   </si>
   <si>
-    <t>Einheit
+    <t xml:space="preserve">Einheit
 Unité</t>
   </si>
   <si>
-    <t>Abgabekategorie Packung
+    <t xml:space="preserve">Abgabekategorie Packung
 Cat. de remise du conditionnement</t>
   </si>
   <si>
-    <t>Abgabekategorie Dosisstärke 
+    <t xml:space="preserve">Abgabekategorie Dosisstärke 
 Cat. de remise du dosage</t>
   </si>
   <si>
-    <t>Abgabekategorie Präparat
+    <t xml:space="preserve">Abgabekategorie Präparat
 Cat. de remise de la préparation</t>
   </si>
   <si>
-    <t>Wirkstoff(e)
+    <t xml:space="preserve">Wirkstoff(e)
 Principe(s) actif(s)</t>
   </si>
   <si>
-    <t>Zusammensetzung
+    <t xml:space="preserve">Zusammensetzung
 Composition</t>
   </si>
   <si>
-    <t>Anwendungsgebiet Präparat
+    <t xml:space="preserve">Anwendungsgebiet Präparat
 Champ d'application de la préparation</t>
   </si>
   <si>
-    <t>Anwendungsgebiet Dosisstärke
+    <t xml:space="preserve">Anwendungsgebiet Dosisstärke
 Champ d'application du dosage</t>
   </si>
   <si>
-    <t>Gentechnisch hergestellte Wirkstoffe
+    <t xml:space="preserve">Gentechnisch hergestellte Wirkstoffe
 Principes actifs produits par génie génétique</t>
   </si>
   <si>
-    <t>Kategorie bei Insulinen
+    <t xml:space="preserve">Kategorie bei Insulinen
 Catégorie en cas d'insuline</t>
   </si>
   <si>
-    <t>Verz. bei betäubunsmittel-haltigen Präparaten** 
+    <t xml:space="preserve">Verz. bei betäubunsmittel-haltigen Präparaten** 
 N° du tabl. si préparations à base de stupéfiants**</t>
   </si>
   <si>
-    <t>Coeur-Vaisseaux Sérocytol, suppositoire</t>
+    <t xml:space="preserve">Coeur-Vaisseaux Sérocytol, suppositoire</t>
   </si>
   <si>
-    <t>Sérolab, société anonyme</t>
+    <t xml:space="preserve">Sérolab, société anonyme</t>
   </si>
   <si>
-    <t>Blutprodukte</t>
+    <t xml:space="preserve">Blutprodukte</t>
   </si>
   <si>
-    <t>08.07.</t>
+    <t xml:space="preserve">08.07.</t>
   </si>
   <si>
-    <t>J06AA</t>
+    <t xml:space="preserve">J06AA</t>
   </si>
   <si>
-    <t>3</t>
+    <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t>Suppositorien</t>
+    <t xml:space="preserve">Suppositorien</t>
   </si>
   <si>
-    <t>B</t>
+    <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t>globulina equina (immunisé avec coeur, endothélium vasculaire porcins)</t>
+    <t xml:space="preserve">globulina equina (immunisé avec coeur, endothélium vasculaire porcins)</t>
   </si>
   <si>
-    <t>globulina equina (immunisé avec coeur, endothélium vasculaire porcins) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
+    <t xml:space="preserve">globulina equina (immunisé avec coeur, endothélium vasculaire porcins) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
   </si>
   <si>
-    <t>Traitement immunomodulant selon le Dr Thomas
+    <t xml:space="preserve">Traitement immunomodulant selon le Dr Thomas
 Possibilités d'emploi voir information professionnelle</t>
   </si>
   <si>
-    <t>9</t>
+    <t xml:space="preserve">9</t>
   </si>
   <si>
-    <t>Colon Sérocytol, suppositoire</t>
+    <t xml:space="preserve">Colon Sérocytol, suppositoire</t>
   </si>
   <si>
-    <t>Sérolab AG</t>
+    <t xml:space="preserve">Sérolab AG</t>
   </si>
   <si>
-    <t>J06A</t>
+    <t xml:space="preserve">J06A</t>
   </si>
   <si>
-    <t>globulina equina (immunisé avec tissu intestinal porcin)</t>
+    <t xml:space="preserve">globulina equina (immunisé avec tissu intestinal porcin)</t>
   </si>
   <si>
-    <t>globulina equina (immunisé avec tissu intestinal porcin) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
+    <t xml:space="preserve">globulina equina (immunisé avec tissu intestinal porcin) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
   </si>
   <si>
-    <t>Traitement immunomodulant  selon le Dr Thomas
+    <t xml:space="preserve">Traitement immunomodulant  selon le Dr Thomas
 Possibilités d'emploi voir information professionnelle</t>
   </si>
   <si>
-    <t>Caniphedrin 20mg ad us.vet., Tabletten</t>
+    <t xml:space="preserve">Caniphedrin 20mg ad us.vet., Tabletten</t>
   </si>
   <si>
-    <t>Streuli Pharma AG</t>
+    <t xml:space="preserve">Streuli Pharma AG</t>
   </si>
   <si>
-    <t>Tierarzneimittel</t>
+    <t xml:space="preserve">Tierarzneimittel</t>
   </si>
   <si>
-    <t>QG04BX90</t>
+    <t xml:space="preserve">QG04BX90</t>
   </si>
   <si>
-    <t>100</t>
+    <t xml:space="preserve">100</t>
   </si>
   <si>
-    <t>Tablette(n)</t>
+    <t xml:space="preserve">Tablette(n)</t>
   </si>
   <si>
-    <t>ephedrini hydrochloridum</t>
+    <t xml:space="preserve">ephedrini hydrochloridum</t>
   </si>
   <si>
-    <t>ephedrini hydrochloridum 20 mg, excipiens pro compresso.</t>
+    <t xml:space="preserve">ephedrini hydrochloridum 20 mg, excipiens pro compresso.</t>
   </si>
   <si>
-    <t>Zur Behandlung der Harninkontinenz bei Hunden</t>
+    <t xml:space="preserve">Zur Behandlung der Harninkontinenz bei Hunden</t>
   </si>
   <si>
-    <t>500</t>
+    <t xml:space="preserve">500</t>
   </si>
   <si>
-    <t>Viscotears Tropfgel, Augengel</t>
+    <t xml:space="preserve">Viscotears Tropfgel, Augengel</t>
   </si>
   <si>
-    <t>Alcon Switzerland SA</t>
+    <t xml:space="preserve">Alcon Switzerland SA</t>
   </si>
   <si>
-    <t>Synthetika human</t>
+    <t xml:space="preserve">Synthetika human</t>
   </si>
   <si>
-    <t>11.08.2.</t>
+    <t xml:space="preserve">11.08.2.</t>
   </si>
   <si>
-    <t>S01XA20</t>
+    <t xml:space="preserve">S01XA20</t>
   </si>
   <si>
-    <t>10</t>
+    <t xml:space="preserve">10</t>
   </si>
   <si>
-    <t>g</t>
+    <t xml:space="preserve">g</t>
   </si>
   <si>
-    <t>D</t>
+    <t xml:space="preserve">D</t>
   </si>
   <si>
-    <t>carbomerum 980</t>
+    <t xml:space="preserve">carbomerum 980</t>
   </si>
   <si>
-    <t>carbomerum 980 2 mg, conserv.: cetrimidum, excipiens ad gelatum pro 1 g.</t>
+    <t xml:space="preserve">carbomerum 980 2 mg, conserv.: cetrimidum, excipiens ad gelatum pro 1 g.</t>
   </si>
   <si>
-    <t>Tränenflüssigkeitsersatz</t>
+    <t xml:space="preserve">Tränenflüssigkeitsersatz</t>
   </si>
   <si>
-    <t>Levetiracetam Desitin 250 mg, Minipacks mit Mini-Filmtabletten</t>
+    <t xml:space="preserve">Levetiracetam Desitin 250 mg, Minipacks mit Mini-Filmtabletten</t>
   </si>
   <si>
-    <t>Desitin Pharma GmbH</t>
+    <t xml:space="preserve">Desitin Pharma GmbH</t>
   </si>
   <si>
-    <t>01.07.1.</t>
+    <t xml:space="preserve">01.07.1.</t>
   </si>
   <si>
-    <t>N03AX14</t>
+    <t xml:space="preserve">N03AX</t>
   </si>
   <si>
-    <t>30</t>
+    <t xml:space="preserve">30</t>
   </si>
   <si>
-    <t>levetiracetamum</t>
+    <t xml:space="preserve">levetiracetamum</t>
   </si>
   <si>
-    <t>levetiracetamum 250 mg, excipiens pro compressi obducti pro charta.</t>
+    <t xml:space="preserve">levetiracetamum 250 mg, excipiens pro compressi obducti pro charta.</t>
   </si>
   <si>
-    <t>Antiepileptikum</t>
+    <t xml:space="preserve">Antiepileptikum</t>
   </si>
   <si>
-    <t>Levetiracetam Desitin 500 mg, Minipacks mit Mini-Filmtabletten</t>
+    <t xml:space="preserve">Levetiracetam Desitin 500 mg, Minipacks mit Mini-Filmtabletten</t>
   </si>
   <si>
-    <t>20</t>
+    <t xml:space="preserve">N03AX14</t>
   </si>
   <si>
-    <t>levetiracetamum 500 mg, excipiens pro compressi obducti pro charta.</t>
+    <t xml:space="preserve">20</t>
   </si>
   <si>
-    <t>200</t>
+    <t xml:space="preserve">levetiracetamum 500 mg, excipiens pro compressi obducti pro charta.</t>
   </si>
   <si>
-    <t>Levetiracetam Desitin 1000 mg, Minipacks mit Mini-Filmtabletten</t>
+    <t xml:space="preserve">200</t>
   </si>
   <si>
-    <t>levetiracetamum 1000 mg, excipiens pro compressi obducti pro charta.</t>
+    <t xml:space="preserve">Levetiracetam Desitin 1000 mg, Minipacks mit Mini-Filmtabletten</t>
   </si>
   <si>
-    <t>Hirudoid, Creme</t>
+    <t xml:space="preserve">levetiracetamum 1000 mg, excipiens pro compressi obducti pro charta.</t>
   </si>
   <si>
-    <t>Medinova AG</t>
+    <t xml:space="preserve">Hirudoid, Creme</t>
   </si>
   <si>
-    <t>02.08.2.</t>
+    <t xml:space="preserve">Medinova AG</t>
   </si>
   <si>
-    <t>C05BA</t>
+    <t xml:space="preserve">02.08.2.</t>
   </si>
   <si>
-    <t>40</t>
+    <t xml:space="preserve">C05BA</t>
   </si>
   <si>
-    <t>heparinoidum (chondroitini polysulfas)</t>
+    <t xml:space="preserve">40</t>
   </si>
   <si>
-    <t>heparinoidum (chondroitini polysulfas) 3 mg alcoholes adipis lanae, aromatica, conserv.: E 218, E 216, excipiens ad unguentum pro 1 g.</t>
+    <t xml:space="preserve">heparinoidum (chondroitini polysulfas)</t>
   </si>
   <si>
-    <t>Venenmittel für den äusserlichen Gebrauch</t>
+    <t xml:space="preserve">heparinoidum (chondroitini polysulfas) 3 mg alcoholes adipis lanae, aromatica, conserv.: E 218, E 216, excipiens ad unguentum pro 1 g.</t>
   </si>
   <si>
-    <t>Amlodipin-Acino  5, Tabletten</t>
+    <t xml:space="preserve">Venenmittel für den äusserlichen Gebrauch</t>
   </si>
   <si>
-    <t>Acino Pharma AG</t>
+    <t xml:space="preserve">Amlodipin-Acino  5, Tabletten</t>
   </si>
   <si>
-    <t>02.06.1.</t>
+    <t xml:space="preserve">Acino Pharma AG</t>
   </si>
   <si>
-    <t>C08CA01</t>
+    <t xml:space="preserve">02.06.1.</t>
   </si>
   <si>
-    <t>amlodipinum</t>
+    <t xml:space="preserve">C08CA01</t>
   </si>
   <si>
-    <t>amlodipinum 5 mg ut amlodipini besilas, excipiens pro compresso.</t>
+    <t xml:space="preserve">amlodipinum</t>
   </si>
   <si>
-    <t>Calciumantagonist</t>
+    <t xml:space="preserve">amlodipinum 5 mg ut amlodipini besilas, excipiens pro compresso.</t>
   </si>
   <si>
-    <t>Hepatect CP, Infusionslösung</t>
+    <t xml:space="preserve">Calciumantagonist</t>
   </si>
   <si>
-    <t>Biotest (Schweiz) AG</t>
+    <t xml:space="preserve">Hepatect CP, Infusionslösung</t>
   </si>
   <si>
-    <t>08.09.</t>
+    <t xml:space="preserve">Biotest (Schweiz) AG</t>
   </si>
   <si>
-    <t>J06BB04</t>
+    <t xml:space="preserve">08.09.</t>
   </si>
   <si>
-    <t>1</t>
+    <t xml:space="preserve">J06BB04</t>
   </si>
   <si>
-    <t>Ampulle(n)</t>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t>immunoglobulinum humanum normale, hepatitidis B virus antigenum</t>
+    <t xml:space="preserve">Ampulle(n)</t>
   </si>
   <si>
-    <t>proteinorum plasmatis humani solutio 50 mg corresp. immunoglobulinum humanum normale min. 96 % et hepatitidis B virus antigenum min. 50 U.I., glycinum, residui: immunoglobulinum A max. 2 mg, aqua q.s. ad solutionem pro 1 ml.</t>
+    <t xml:space="preserve">immunoglobulinum humanum normale, hepatitidis B virus antigenum</t>
   </si>
   <si>
-    <t>passive Immunisierung gegen Hepatitis B</t>
+    <t xml:space="preserve">proteinorum plasmatis humani solutio 50 mg corresp. immunoglobulinum humanum normale min. 96 % et hepatitidis B virus antigenum min. 50 U.I., glycinum, residui: immunoglobulinum A max. 2 mg, aqua q.s. ad solutionem pro 1 ml.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passive Immunisierung gegen Hepatitis B</t>
   </si>
 </sst>
 </file>
@@ -393,7 +407,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY;@"/>
     <numFmt numFmtId="166" formatCode="00000"/>
     <numFmt numFmtId="167" formatCode="000"/>
@@ -557,7 +571,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -577,7 +591,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -585,71 +599,71 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -669,20 +683,44 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -705,8 +743,8 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -733,41 +771,17 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Standard 2" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Standard 2" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Standard 2" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Standard 2" xfId="20"/>
+    <cellStyle name="Excel Built-in Excel Built-in Standard 2" xfId="21"/>
+    <cellStyle name="Excel Built-in Standard 2" xfId="22"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -783,9 +797,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1069200</xdr:colOff>
+      <xdr:colOff>1068840</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>28440</xdr:rowOff>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -799,7 +813,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="119520" y="360"/>
-          <a:ext cx="1692360" cy="561240"/>
+          <a:ext cx="1692000" cy="560880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -819,31 +833,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:22"/>
+  <dimension ref="A1:AMJ22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="6.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.06632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="4.46428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="57.4336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.0510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.65816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.5408163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="11.25"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="4.9030612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.2397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="3" width="31.8826530612245"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="5.91326530612245"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="56.1275510204082"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="33.1785714285714"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="36.7908163265306"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="59.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="2" width="6.91836734693878"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="57.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="1" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="31.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="5.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="56.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="33.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="36.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="59.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="19" style="2" width="6.92"/>
   </cols>
   <sheetData>
     <row r="1" s="12" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9550,7 +9564,7 @@
         <v>67</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H14" s="39" t="n">
         <v>40610</v>
@@ -9565,7 +9579,7 @@
         <v>9</v>
       </c>
       <c r="L14" s="37" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M14" s="37" t="s">
         <v>49</v>
@@ -9583,7 +9597,7 @@
         <v>70</v>
       </c>
       <c r="R14" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S14" s="38" t="s">
         <v>72</v>
@@ -10614,7 +10628,7 @@
         <v>67</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H15" s="39" t="n">
         <v>40610</v>
@@ -10647,7 +10661,7 @@
         <v>70</v>
       </c>
       <c r="R15" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S15" s="38" t="s">
         <v>72</v>
@@ -11678,7 +11692,7 @@
         <v>67</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H16" s="39" t="n">
         <v>40610</v>
@@ -11693,7 +11707,7 @@
         <v>11</v>
       </c>
       <c r="L16" s="37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M16" s="37" t="s">
         <v>49</v>
@@ -11711,7 +11725,7 @@
         <v>70</v>
       </c>
       <c r="R16" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S16" s="38" t="s">
         <v>72</v>
@@ -12730,7 +12744,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D17" s="38" t="s">
         <v>66</v>
@@ -12742,7 +12756,7 @@
         <v>67</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H17" s="39" t="n">
         <v>40610</v>
@@ -12775,7 +12789,7 @@
         <v>70</v>
       </c>
       <c r="R17" s="38" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="S17" s="38" t="s">
         <v>72</v>
@@ -13794,7 +13808,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D18" s="38" t="s">
         <v>66</v>
@@ -13806,7 +13820,7 @@
         <v>67</v>
       </c>
       <c r="G18" s="37" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H18" s="39" t="n">
         <v>40610</v>
@@ -13839,7 +13853,7 @@
         <v>70</v>
       </c>
       <c r="R18" s="38" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="S18" s="38" t="s">
         <v>72</v>
@@ -14858,7 +14872,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D19" s="38" t="s">
         <v>66</v>
@@ -14870,7 +14884,7 @@
         <v>67</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H19" s="39" t="n">
         <v>40610</v>
@@ -14885,7 +14899,7 @@
         <v>14</v>
       </c>
       <c r="L19" s="37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M19" s="37" t="s">
         <v>49</v>
@@ -14903,7 +14917,7 @@
         <v>70</v>
       </c>
       <c r="R19" s="38" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="S19" s="38" t="s">
         <v>72</v>
@@ -15922,19 +15936,19 @@
         <v>1</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E20" s="38" t="s">
         <v>56</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H20" s="39" t="n">
         <v>18872</v>
@@ -15949,7 +15963,7 @@
         <v>58</v>
       </c>
       <c r="L20" s="37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M20" s="37" t="s">
         <v>60</v>
@@ -15964,13 +15978,13 @@
         <v>61</v>
       </c>
       <c r="Q20" s="38" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="R20" s="38" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S20" s="38" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="T20" s="38"/>
       <c r="U20" s="37"/>
@@ -16986,19 +17000,19 @@
         <v>3</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" s="44" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E21" s="44" t="s">
         <v>56</v>
       </c>
       <c r="F21" s="43" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G21" s="43" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H21" s="45" t="n">
         <v>39213</v>
@@ -17028,13 +17042,13 @@
         <v>33</v>
       </c>
       <c r="Q21" s="44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R21" s="44" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="S21" s="44" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="T21" s="44"/>
       <c r="U21" s="43"/>
@@ -17049,19 +17063,19 @@
         <v>2</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D22" s="50" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E22" s="50" t="s">
         <v>28</v>
       </c>
       <c r="F22" s="49" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G22" s="49" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H22" s="51" t="n">
         <v>29995</v>
@@ -17076,10 +17090,10 @@
         <v>1</v>
       </c>
       <c r="L22" s="49" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M22" s="49" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N22" s="49" t="s">
         <v>33</v>
@@ -17091,13 +17105,13 @@
         <v>33</v>
       </c>
       <c r="Q22" s="50" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="R22" s="50" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="S22" s="50" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="T22" s="50"/>
       <c r="U22" s="49"/>
@@ -17110,7 +17124,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.279861111111111" bottom="0.490277777777778" header="0.511805555555555" footer="0"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;CSwissmedic · Hallerstrasse 7 · CH-3000 Bern 9 · www.swissmedic.ch · Tel. +41 31 322 02 11 · Fax +41 31 322 02 12&amp;R&amp;P/&amp;N</oddFooter>

</xml_diff>